<commit_message>
codigo do generate_certificate.py atualizado. Foi colocado um limite de caracteres para cada nome
</commit_message>
<xml_diff>
--- a/lista_alunos.xlsx
+++ b/lista_alunos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renan\OneDrive\Área de Trabalho\PycharmProjects\Gerador-De-Certificados---IEEE-UFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F5BC9F-AC50-4D77-87BE-512DC4C49FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F4AF1F-93C7-4421-B471-5A107EE45A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2556" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <t>renan_sn@id.uff.br</t>
   </si>
   <si>
-    <t>RENAN SOUZA DO NASCIMENTO</t>
+    <t>RENAN SOUZA DA SILVA FERREIRA DO NASCIMENTO</t>
   </si>
 </sst>
 </file>
@@ -388,7 +388,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
generate_certificate.py atualizado. tamanho_maximo diminuido
</commit_message>
<xml_diff>
--- a/lista_alunos.xlsx
+++ b/lista_alunos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renan\OneDrive\Área de Trabalho\PycharmProjects\Gerador-De-Certificados---IEEE-UFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F4AF1F-93C7-4421-B471-5A107EE45A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E639BB7-EED8-4EFD-ADED-37B15594B88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2556" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,10 +385,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -413,6 +413,9 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{B0E2F2B5-660D-4B6F-A667-9B5C6B6E74DB}"/>

</xml_diff>